<commit_message>
update with horizontal and vertical layout
</commit_message>
<xml_diff>
--- a/swimmer.xlsx
+++ b/swimmer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pgrogan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stevens0-my.sharepoint.com/personal/pgrogan_stevens_edu/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB821F6B-F16C-4F6C-895A-87B47D7BB663}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="13_ncr:1_{FB821F6B-F16C-4F6C-895A-87B47D7BB663}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{08564858-20DC-4112-9908-69147669C011}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="660" windowWidth="25236" windowHeight="19656" xr2:uid="{ACB790FA-54D0-41FA-ACF1-70957FC8ADEA}"/>
+    <workbookView xWindow="3420" yWindow="3495" windowWidth="43200" windowHeight="23535" xr2:uid="{ACB790FA-54D0-41FA-ACF1-70957FC8ADEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>Start Date</t>
   </si>
@@ -44,16 +44,7 @@
     <t>End</t>
   </si>
   <si>
-    <t>Patient</t>
-  </si>
-  <si>
     <t>Biopsy</t>
-  </si>
-  <si>
-    <t>Biopsy Date</t>
-  </si>
-  <si>
-    <t>Transplant Date</t>
   </si>
   <si>
     <t>Transplant</t>
@@ -65,7 +56,10 @@
     <t>Treatment</t>
   </si>
   <si>
-    <t>Treatment Date</t>
+    <t>Patient ID</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -75,7 +69,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,13 +80,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF0070C0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -118,13 +105,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2403,7 +2389,2308 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v/>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="minus"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="100"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="50800" cap="flat" cmpd="sng" algn="ctr">
+                <a:noFill/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="minus"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="100"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="50800" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$100</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="99"/>
+                <c:pt idx="0">
+                  <c:v>20.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$100</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="99"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8BB9-48B2-A8E4-5E1C3DCD1558}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Treatment</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="9"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$2:$I$100</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="99"/>
+                <c:pt idx="0">
+                  <c:v>2.6666666666666665</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0333333333333332</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.0666666666666664</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.833333333333334</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.1333333333333329</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$100</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="99"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8BB9-48B2-A8E4-5E1C3DCD1558}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Biopsy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$M$2:$M$100</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="99"/>
+                <c:pt idx="0">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.866666666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$2:$K$100</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="99"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8BB9-48B2-A8E4-5E1C3DCD1558}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Transplant</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$Q$2:$Q$100</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="99"/>
+                <c:pt idx="0">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$O$2:$O$100</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="99"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-8BB9-48B2-A8E4-5E1C3DCD1558}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v/>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="plus"/>
+            <c:errValType val="fixedVal"/>
+            <c:noEndCap val="1"/>
+            <c:val val="2"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+                <a:noFill/>
+                <a:round/>
+                <a:headEnd type="none"/>
+                <a:tailEnd type="stealth"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="plus"/>
+            <c:errValType val="fixedVal"/>
+            <c:noEndCap val="1"/>
+            <c:val val="1"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:round/>
+                <a:tailEnd type="stealth"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$T$2:$T$100</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="99"/>
+                <c:pt idx="0">
+                  <c:v>20.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$S$2:$S$100</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="99"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-8BB9-48B2-A8E4-5E1C3DCD1558}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1396594575"/>
+        <c:axId val="1525449167"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1396594575"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Months</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1525449167"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1525449167"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+          <c:max val="22.5"/>
+          <c:min val="0.5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Patient</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:noFill/>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1396594575"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2959,20 +5246,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>15904</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
+      <xdr:colOff>40752</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>56320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>270890</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>39756</xdr:rowOff>
+      <xdr:colOff>295738</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>172277</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2994,6 +5797,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>49695</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>49694</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>314738</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>150742</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0632D86B-39DE-408A-80A5-54CEBD4C022C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3302,25 +6143,32 @@
   <dimension ref="A1:T100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.21875" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.109375" style="2"/>
-    <col min="13" max="13" width="9.109375" style="2"/>
-    <col min="17" max="17" width="8.88671875" style="2"/>
-    <col min="20" max="20" width="9.109375" style="2"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -3332,40 +6180,40 @@
         <v>2</v>
       </c>
       <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="S1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="O1" t="s">
-        <v>3</v>
-      </c>
-      <c r="P1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="S1" t="s">
-        <v>3</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3418,7 +6266,7 @@
         <v>20.9</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3467,7 +6315,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3508,11 +6356,11 @@
         <v>10</v>
       </c>
       <c r="T4" s="2">
-        <f t="shared" ref="T3:T66" si="4">IF(ISBLANK(S4),,VLOOKUP(S4,$A:$D,4))</f>
+        <f t="shared" ref="T4:T66" si="4">IF(ISBLANK(S4),,VLOOKUP(S4,$A:$D,4))</f>
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3557,7 +6405,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3598,7 +6446,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3633,7 +6481,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3665,7 +6513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3697,7 +6545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3729,7 +6577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3761,7 +6609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3793,7 +6641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3825,7 +6673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3857,7 +6705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3889,7 +6737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3921,7 +6769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3953,7 +6801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3985,7 +6833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4017,7 +6865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4049,7 +6897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4081,7 +6929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4113,7 +6961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -4145,7 +6993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="2">
@@ -4170,7 +7018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="2">
@@ -4195,7 +7043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C26" s="1"/>
       <c r="D26" s="2">
         <f>IF(ISBLANK(C26),,(C26-B26)/30)</f>
@@ -4218,7 +7066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D27" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4240,7 +7088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D28" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4262,7 +7110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D29" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4284,7 +7132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D30" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4306,7 +7154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D31" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4328,7 +7176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D32" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4350,7 +7198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D33" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4372,7 +7220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D34" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4394,7 +7242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D35" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4416,7 +7264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D36" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4438,7 +7286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D37" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4460,7 +7308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D38" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4482,7 +7330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D39" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4504,7 +7352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D40" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4526,7 +7374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D41" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4548,7 +7396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D42" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4570,7 +7418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D43" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4592,7 +7440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D44" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4614,7 +7462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D45" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4636,7 +7484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D46" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4658,7 +7506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D47" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4680,7 +7528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D48" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4702,7 +7550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D49" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4724,7 +7572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D50" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4746,7 +7594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D51" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4768,7 +7616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D52" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4790,7 +7638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D53" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4812,7 +7660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="54" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D54" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4834,7 +7682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="55" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D55" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4856,7 +7704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="56" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D56" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4878,7 +7726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="57" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D57" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4900,7 +7748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="58" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D58" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4922,7 +7770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="59" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D59" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4944,7 +7792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="60" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D60" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4966,7 +7814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="61" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D61" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4988,7 +7836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="62" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D62" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5010,7 +7858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="63" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D63" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5032,7 +7880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="64" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D64" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5054,7 +7902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="65" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D65" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5076,7 +7924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="66" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D66" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5098,7 +7946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="67" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D67" s="2">
         <f t="shared" ref="D67:D100" si="5">IF(ISBLANK(C67),,(C67-B67)/30)</f>
         <v>0</v>
@@ -5120,7 +7968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="68" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D68" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5142,7 +7990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="69" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D69" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5164,7 +8012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="70" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D70" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5186,7 +8034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="71" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D71" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5208,7 +8056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="72" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D72" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5230,7 +8078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="73" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D73" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5252,7 +8100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="74" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D74" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5274,7 +8122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="75" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D75" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5296,7 +8144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="76" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D76" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5318,7 +8166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="77" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D77" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5340,7 +8188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="78" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D78" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5362,7 +8210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="79" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D79" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5384,7 +8232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="80" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D80" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5406,7 +8254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="81" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D81" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5428,7 +8276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="82" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D82" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5450,7 +8298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="83" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D83" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5472,7 +8320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="84" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D84" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5494,7 +8342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="85" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D85" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5516,7 +8364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="86" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D86" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5538,7 +8386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="87" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D87" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5560,7 +8408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="88" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D88" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5582,7 +8430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="89" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D89" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5604,7 +8452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="90" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D90" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5626,7 +8474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="91" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D91" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5648,7 +8496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="92" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D92" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5670,7 +8518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="93" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D93" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5692,7 +8540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="94" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D94" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5714,7 +8562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="95" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D95" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5736,7 +8584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="96" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D96" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5758,7 +8606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="97" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D97" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5780,7 +8628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="98" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D98" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5802,7 +8650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="99" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D99" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5824,7 +8672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="100" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D100" s="2">
         <f t="shared" si="5"/>
         <v>0</v>

</xml_diff>